<commit_message>
07.11.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Price list 28-10-2020.xlsx
+++ b/2020/Others/Price list 28-10-2020.xlsx
@@ -288,7 +288,7 @@
     <t>T130</t>
   </si>
   <si>
-    <t>Last Update(03-11-2020)</t>
+    <t>Last Update(05-11-2020)</t>
   </si>
 </sst>
 </file>
@@ -639,7 +639,7 @@
         <xdr:cNvPr id="2" name="Group 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -660,7 +660,7 @@
           <xdr:cNvPr id="3" name="Freeform 21">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -866,7 +866,7 @@
           <xdr:cNvPr id="4" name="Freeform 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1967,7 +1967,7 @@
           <xdr:cNvPr id="5" name="Freeform 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2414,7 +2414,7 @@
           <xdr:cNvPr id="6" name="Freeform 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2474,7 +2474,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2491,7 +2491,7 @@
           <xdr:cNvPr id="7" name="Freeform 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2554,7 +2554,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2571,7 +2571,7 @@
           <xdr:cNvPr id="8" name="Freeform 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2631,7 +2631,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2664,7 +2664,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2676,7 +2676,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2954,7 +2954,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2965,7 +2965,7 @@
   <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>